<commit_message>
Add/Edit logic, discount class, small fixes
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -219,21 +219,6 @@
     <t>Сергеевич</t>
   </si>
   <si>
-    <t xml:space="preserve"> Кемеровская область</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Архангельская область</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ленинградская область</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Московская область</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Белгородская область</t>
-  </si>
-  <si>
     <t>Юрга</t>
   </si>
   <si>
@@ -277,6 +262,21 @@
   </si>
   <si>
     <t>HouseNum</t>
+  </si>
+  <si>
+    <t>Ленинградская область</t>
+  </si>
+  <si>
+    <t>Архангельская область</t>
+  </si>
+  <si>
+    <t>Белгородская область</t>
+  </si>
+  <si>
+    <t>Кемеровская область</t>
+  </si>
+  <si>
+    <t>Московская область</t>
   </si>
 </sst>
 </file>
@@ -708,15 +708,16 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1353,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1360,7 +1361,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1368,7 +1369,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1376,7 +1377,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1402,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1410,7 +1411,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1418,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,7 +1427,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1434,7 +1435,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1471,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1479,7 +1480,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1487,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1495,7 +1496,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1553,19 +1554,19 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="K1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N1" t="s">
         <v>15</v>
@@ -1811,11 +1812,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1"/>
-    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
     <hyperlink ref="G4" r:id="rId3"/>
-    <hyperlink ref="G3" r:id="rId4"/>
-    <hyperlink ref="G2" r:id="rId5"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>